<commit_message>
update text and files
lots of updates
</commit_message>
<xml_diff>
--- a/data/Min_Traffic_Death_Rate.xlsx
+++ b/data/Min_Traffic_Death_Rate.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pinkgold/Documents/developer/choropleth_map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{907831DE-F1DD-C14B-B21A-F53DE375C904}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7E6236-2820-0C4A-AD74-DB5A084F6C57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Min_Traffic_Death_Rate" sheetId="1" r:id="rId1"/>
@@ -631,7 +631,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1465,14 +1465,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I1" sqref="H1:I1048576"/>
+      <selection activeCell="K29" sqref="K29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="18.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
added screenshots and clarrifying text
happy now
</commit_message>
<xml_diff>
--- a/data/Min_Traffic_Death_Rate.xlsx
+++ b/data/Min_Traffic_Death_Rate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pinkgold/Documents/developer/choropleth_map/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB7E6236-2820-0C4A-AD74-DB5A084F6C57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A969F848-A32B-104D-AC7C-6667AE2A0470}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Min_Traffic_Death_Rate" sheetId="1" r:id="rId1"/>
@@ -1109,8 +1109,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1469,40 +1470,41 @@
   <dimension ref="A1:I196"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
     <col min="3" max="3" width="18.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1">
+      <c r="E1" s="1">
         <v>2000</v>
       </c>
-      <c r="F1">
+      <c r="F1" s="1">
         <v>2005</v>
       </c>
-      <c r="G1">
+      <c r="G1" s="1">
         <v>2010</v>
       </c>
-      <c r="H1">
+      <c r="H1" s="1">
         <v>2013</v>
       </c>
-      <c r="I1">
+      <c r="I1" s="1">
         <v>2016</v>
       </c>
     </row>

</xml_diff>